<commit_message>
Update Tuned_Parameters CHN Paper.xlsx
</commit_message>
<xml_diff>
--- a/Data_Learning_Prediction/For_Paper_Result_Plots/Tuned_Parameters CHN Paper.xlsx
+++ b/Data_Learning_Prediction/For_Paper_Result_Plots/Tuned_Parameters CHN Paper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murat.ozemre\Desktop\Thesis_Project\Data_Learning_Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murat.ozemre\Desktop\Thesis_Project\Data_Learning_Prediction\For_Paper_Result_Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,11 +16,33 @@
     <sheet name="NN" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$D$7</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2:$B$7</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet2!$A$2:$B$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet2!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet2!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet2!$A$2:$B$7</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet2!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet2!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet2!$A$2:$B$7</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet2!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet2!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$A$2:$B$7</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet2!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet2!$D$2:$D$7</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -320,90 +342,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="tr-TR"/>
-              <a:t> After</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="tr-TR" baseline="0"/>
-              <a:t> Tuning RF and NN Models  </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="tr-TR" baseline="0"/>
-              <a:t>R2 Results (median values</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="tr-TR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -426,7 +372,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -734,7 +682,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1148,7 +1098,868 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> After</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR" baseline="0"/>
+              <a:t> Tuning RF and NN Models  </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="tr-TR" baseline="0"/>
+              <a:t>R2 Results (median values</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Same Set</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-1.548586914440573E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.0177781169293865E-17"/>
+                  <c:y val="-1.5485869144405695E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.7100271002710029E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1915406530791147E-3"/>
+                  <c:y val="-1.5485869144405801E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0957703265395573E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.7532325224632918E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$A$2:$B$7</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>RF</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NN</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>RF</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NN</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>RF</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NN</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>841810</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>841810</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>841840</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>841840</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>841850</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>841850</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.65100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.374</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53550000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9225000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80200000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E98F-4473-B116-237BA4511FCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Different Set</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1915406530790943E-3"/>
+                  <c:y val="1.1614401858304263E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.5746219592373442E-3"/>
+                  <c:y val="-3.5488040161728201E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.5746219592373442E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-E98F-4473-B116-237BA4511FCC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$A$2:$B$7</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>RF</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NN</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>RF</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NN</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>RF</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NN</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>841810</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>841810</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>841840</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>841840</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>841850</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>841850</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.65500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.374</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-E98F-4473-B116-237BA4511FCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="619855632"/>
+        <c:axId val="619856288"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="619855632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619856288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="619856288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619855632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1189,6 +2000,509 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1725,123 +3039,39 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="RF"/>
-      <sheetName val="NN"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Summary,"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Results from NN and RF"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>Same Set</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Different Set</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>841810</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>RF</v>
-          </cell>
-          <cell r="C2">
-            <v>0.72599999999999998</v>
-          </cell>
-          <cell r="D2">
-            <v>0.72599999999999998</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>841810</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>NN</v>
-          </cell>
-          <cell r="C3">
-            <v>0.67500000000000004</v>
-          </cell>
-          <cell r="D3">
-            <v>0.70499999999999996</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>841840</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>RF</v>
-          </cell>
-          <cell r="C4">
-            <v>0.65</v>
-          </cell>
-          <cell r="D4">
-            <v>0.64900000000000002</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>841840</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>NN</v>
-          </cell>
-          <cell r="C5">
-            <v>0.45900000000000002</v>
-          </cell>
-          <cell r="D5">
-            <v>0.441</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>841850</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>RF</v>
-          </cell>
-          <cell r="C6">
-            <v>0.94</v>
-          </cell>
-          <cell r="D6">
-            <v>0.94</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>841850</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>NN</v>
-          </cell>
-          <cell r="C7">
-            <v>0.88600000000000001</v>
-          </cell>
-          <cell r="D7">
-            <v>0.878</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3259,8 +4489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>